<commit_message>
updated version to 0.5.0-pre-230703-2
</commit_message>
<xml_diff>
--- a/docs/NDependStatistics.xlsx
+++ b/docs/NDependStatistics.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Shared\PayrollEngine\Repos\PayrollEngine\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Shared\PayrollEngine\Repos\PayrollEngine\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D1C36E1-E0B0-49B2-BB0F-6136694CB019}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C884B9B0-0B19-4E0F-9073-B4745F79732A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19590" yWindow="5030" windowWidth="16950" windowHeight="12570" xr2:uid="{2F54338B-7147-491F-9A14-A030957DD08E}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{2F54338B-7147-491F-9A14-A030957DD08E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,9 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>tc={66ED0313-C67B-4B7A-BA6A-9A7B81063671}</author>
+    <author>tc={3AEE2784-2DD4-43F8-BE44-B0BFB5F45216}</author>
     <author>tc={41DF860C-BD5B-4123-B2C9-32E84BDF1D2B}</author>
+    <author>tc={54FB35DA-D397-480C-B479-997CCF72697B}</author>
   </authors>
   <commentList>
     <comment ref="I10" authorId="0" shapeId="0" xr:uid="{66ED0313-C67B-4B7A-BA6A-9A7B81063671}">
@@ -50,7 +52,23 @@
     2 days for [A]</t>
       </text>
     </comment>
-    <comment ref="I12" authorId="1" shapeId="0" xr:uid="{41DF860C-BD5B-4123-B2C9-32E84BDF1D2B}">
+    <comment ref="S10" authorId="1" shapeId="0" xr:uid="{3AEE2784-2DD4-43F8-BE44-B0BFB5F45216}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    2 days for [A]</t>
+      </text>
+    </comment>
+    <comment ref="I12" authorId="2" shapeId="0" xr:uid="{41DF860C-BD5B-4123-B2C9-32E84BDF1D2B}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    1 hour to [A]</t>
+      </text>
+    </comment>
+    <comment ref="S12" authorId="3" shapeId="0" xr:uid="{54FB35DA-D397-480C-B479-997CCF72697B}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -63,7 +81,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="25">
   <si>
     <t>Repository</t>
   </si>
@@ -92,9 +110,6 @@
     <t>Dev Effort (Days)</t>
   </si>
   <si>
-    <t>Vialated Rules</t>
-  </si>
-  <si>
     <t>Debt Effort (Days)</t>
   </si>
   <si>
@@ -137,7 +152,10 @@
     <t>Total</t>
   </si>
   <si>
-    <t>Last Update</t>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Violated Rules</t>
   </si>
 </sst>
 </file>
@@ -147,7 +165,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -185,6 +203,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -237,7 +261,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -274,6 +298,12 @@
     </xf>
     <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -598,7 +628,13 @@
   <threadedComment ref="I10" dT="2023-05-24T06:37:35.39" personId="{62F06B25-A6F5-4F82-AFC4-F7A67E88A8A3}" id="{66ED0313-C67B-4B7A-BA6A-9A7B81063671}">
     <text>2 days for [A]</text>
   </threadedComment>
+  <threadedComment ref="S10" dT="2023-05-24T06:37:35.39" personId="{62F06B25-A6F5-4F82-AFC4-F7A67E88A8A3}" id="{3AEE2784-2DD4-43F8-BE44-B0BFB5F45216}">
+    <text>2 days for [A]</text>
+  </threadedComment>
   <threadedComment ref="I12" dT="2023-05-24T06:40:01.82" personId="{62F06B25-A6F5-4F82-AFC4-F7A67E88A8A3}" id="{41DF860C-BD5B-4123-B2C9-32E84BDF1D2B}">
+    <text>1 hour to [A]</text>
+  </threadedComment>
+  <threadedComment ref="S12" dT="2023-05-24T06:40:01.82" personId="{62F06B25-A6F5-4F82-AFC4-F7A67E88A8A3}" id="{54FB35DA-D397-480C-B479-997CCF72697B}">
     <text>1 hour to [A]</text>
   </threadedComment>
 </ThreadedComments>
@@ -606,10 +642,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91D4D49F-38D9-40C5-817A-D2EA74B5A307}">
-  <dimension ref="B1:J19"/>
+  <dimension ref="B1:T19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:C3"/>
+      <selection activeCell="M5" sqref="M5:T5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -621,68 +657,109 @@
     <col min="5" max="6" width="15.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="16" style="1" customWidth="1"/>
     <col min="9" max="9" width="17.453125" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="8.7265625" style="1"/>
+    <col min="10" max="11" width="8.7265625" style="1"/>
+    <col min="12" max="12" width="37.26953125" style="1" customWidth="1"/>
+    <col min="13" max="13" width="11.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.90625" style="1" customWidth="1"/>
+    <col min="15" max="16" width="15.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="16" style="1" customWidth="1"/>
+    <col min="19" max="19" width="17.453125" style="1" customWidth="1"/>
+    <col min="20" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" ht="9.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:10" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:20" ht="9.5" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:20" ht="49.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B2" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="L2" s="2"/>
+    </row>
+    <row r="3" spans="2:20" x14ac:dyDescent="0.35">
       <c r="B3" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="12">
+        <v>45111</v>
+      </c>
+      <c r="L3" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="M3" s="12">
+        <v>45070</v>
+      </c>
+    </row>
+    <row r="4" spans="2:20" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="5" spans="2:20" ht="23.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B5" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="G5" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="H5" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="12">
-        <v>45070</v>
-      </c>
-    </row>
-    <row r="4" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="5" spans="2:10" ht="23.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B5" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C5" s="3" t="s">
+      <c r="I5" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="J5" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="M5" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="N5" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="O5" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="P5" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="Q5" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="R5" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="S5" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="I5" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="J5" s="3" t="s">
+      <c r="T5" s="14" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="2:10" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:20" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B6" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C6" s="6">
-        <v>2195</v>
+        <v>2279</v>
       </c>
       <c r="D6" s="6">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E6" s="6">
         <v>52</v>
       </c>
       <c r="F6" s="6">
-        <v>2387</v>
+        <v>2279</v>
       </c>
       <c r="G6" s="6">
         <v>1</v>
@@ -694,12 +771,39 @@
         <v>1</v>
       </c>
       <c r="J6" s="6">
+        <v>1.56</v>
+      </c>
+      <c r="L6" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="M6" s="6">
+        <v>2195</v>
+      </c>
+      <c r="N6" s="6">
+        <v>65</v>
+      </c>
+      <c r="O6" s="6">
+        <v>52</v>
+      </c>
+      <c r="P6" s="6">
+        <v>2387</v>
+      </c>
+      <c r="Q6" s="6">
+        <v>1</v>
+      </c>
+      <c r="R6" s="6">
+        <v>8</v>
+      </c>
+      <c r="S6" s="6">
+        <v>1</v>
+      </c>
+      <c r="T6" s="6">
         <v>1.61</v>
       </c>
     </row>
-    <row r="7" spans="2:10" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:20" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B7" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C7" s="1">
         <v>86</v>
@@ -725,10 +829,37 @@
       <c r="J7" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="2:10" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="L7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M7" s="1">
+        <v>86</v>
+      </c>
+      <c r="N7" s="1">
+        <v>2</v>
+      </c>
+      <c r="O7" s="1">
+        <v>35</v>
+      </c>
+      <c r="P7" s="1">
+        <v>46</v>
+      </c>
+      <c r="Q7" s="1">
+        <v>0</v>
+      </c>
+      <c r="R7" s="1">
+        <v>0</v>
+      </c>
+      <c r="S7" s="1">
+        <v>0</v>
+      </c>
+      <c r="T7" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="2:20" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B8" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C8" s="1">
         <v>18</v>
@@ -754,51 +885,105 @@
       <c r="J8" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="2:10" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="L8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M8" s="1">
+        <v>18</v>
+      </c>
+      <c r="N8" s="1">
+        <v>1</v>
+      </c>
+      <c r="O8" s="1">
+        <v>84</v>
+      </c>
+      <c r="P8" s="1">
+        <v>93</v>
+      </c>
+      <c r="Q8" s="1">
+        <v>0</v>
+      </c>
+      <c r="R8" s="1">
+        <v>0</v>
+      </c>
+      <c r="S8" s="1">
+        <v>0</v>
+      </c>
+      <c r="T8" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="2:20" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B9" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C9" s="1">
-        <v>6823</v>
+        <v>7174</v>
       </c>
       <c r="D9" s="1">
-        <v>248</v>
+        <v>258</v>
       </c>
       <c r="E9" s="1">
         <v>36</v>
       </c>
       <c r="F9" s="1">
-        <v>3813</v>
+        <v>3936</v>
       </c>
       <c r="G9" s="1">
         <v>3</v>
       </c>
       <c r="H9" s="1">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I9" s="1">
         <v>11</v>
       </c>
       <c r="J9" s="1">
+        <v>4.51</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="M9" s="1">
+        <v>6823</v>
+      </c>
+      <c r="N9" s="1">
+        <v>248</v>
+      </c>
+      <c r="O9" s="1">
+        <v>36</v>
+      </c>
+      <c r="P9" s="1">
+        <v>3813</v>
+      </c>
+      <c r="Q9" s="1">
+        <v>3</v>
+      </c>
+      <c r="R9" s="1">
+        <v>13</v>
+      </c>
+      <c r="S9" s="1">
+        <v>11</v>
+      </c>
+      <c r="T9" s="1">
         <v>4.5199999999999996</v>
       </c>
     </row>
-    <row r="10" spans="2:10" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:20" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B10" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C10" s="1">
-        <v>6226</v>
+        <v>6296</v>
       </c>
       <c r="D10" s="1">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="E10" s="1">
         <v>48</v>
       </c>
       <c r="F10" s="1">
-        <v>5700</v>
+        <v>5665</v>
       </c>
       <c r="G10" s="1">
         <v>4</v>
@@ -810,24 +995,51 @@
         <v>11</v>
       </c>
       <c r="J10" s="4">
+        <v>6.42</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="M10" s="1">
+        <v>6226</v>
+      </c>
+      <c r="N10" s="1">
+        <v>185</v>
+      </c>
+      <c r="O10" s="1">
+        <v>48</v>
+      </c>
+      <c r="P10" s="1">
+        <v>5700</v>
+      </c>
+      <c r="Q10" s="1">
+        <v>4</v>
+      </c>
+      <c r="R10" s="1">
+        <v>15</v>
+      </c>
+      <c r="S10" s="1">
+        <v>11</v>
+      </c>
+      <c r="T10" s="4">
         <v>6.36</v>
       </c>
     </row>
-    <row r="11" spans="2:10" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:20" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B11" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C11" s="1">
-        <v>1159</v>
+        <v>1201</v>
       </c>
       <c r="D11" s="1">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E11" s="1">
         <v>40</v>
       </c>
       <c r="F11" s="1">
-        <v>787</v>
+        <v>801</v>
       </c>
       <c r="G11" s="1">
         <v>2</v>
@@ -839,15 +1051,42 @@
         <v>1</v>
       </c>
       <c r="J11" s="1">
+        <v>4.7699999999999996</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="M11" s="1">
+        <v>1159</v>
+      </c>
+      <c r="N11" s="1">
+        <v>32</v>
+      </c>
+      <c r="O11" s="1">
+        <v>40</v>
+      </c>
+      <c r="P11" s="1">
+        <v>787</v>
+      </c>
+      <c r="Q11" s="1">
+        <v>2</v>
+      </c>
+      <c r="R11" s="1">
+        <v>4</v>
+      </c>
+      <c r="S11" s="1">
+        <v>1</v>
+      </c>
+      <c r="T11" s="1">
         <v>4.9000000000000004</v>
       </c>
     </row>
-    <row r="12" spans="2:10" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:20" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B12" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C12" s="1">
-        <v>1707</v>
+        <v>1713</v>
       </c>
       <c r="D12" s="1">
         <v>47</v>
@@ -856,65 +1095,119 @@
         <v>43</v>
       </c>
       <c r="F12" s="1">
-        <v>1269</v>
+        <v>1281</v>
       </c>
       <c r="G12" s="1">
         <v>2</v>
       </c>
       <c r="H12" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I12" s="1">
         <v>2</v>
       </c>
       <c r="J12" s="4">
+        <v>5.26</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="M12" s="1">
+        <v>1707</v>
+      </c>
+      <c r="N12" s="1">
+        <v>47</v>
+      </c>
+      <c r="O12" s="1">
+        <v>43</v>
+      </c>
+      <c r="P12" s="1">
+        <v>1269</v>
+      </c>
+      <c r="Q12" s="1">
+        <v>2</v>
+      </c>
+      <c r="R12" s="1">
+        <v>8</v>
+      </c>
+      <c r="S12" s="1">
+        <v>2</v>
+      </c>
+      <c r="T12" s="4">
         <v>5.31</v>
       </c>
     </row>
-    <row r="13" spans="2:10" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:20" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B13" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C13" s="1">
-        <v>18189</v>
+        <v>18550</v>
       </c>
       <c r="D13" s="1">
-        <v>577</v>
+        <v>585</v>
       </c>
       <c r="E13" s="1">
         <v>43</v>
       </c>
       <c r="F13" s="1">
-        <v>13990</v>
+        <v>14209</v>
       </c>
       <c r="G13" s="1">
         <v>4</v>
       </c>
       <c r="H13" s="1">
+        <v>14</v>
+      </c>
+      <c r="I13" s="1">
         <v>15</v>
       </c>
-      <c r="I13" s="1">
+      <c r="J13" s="1">
+        <v>2.66</v>
+      </c>
+      <c r="L13" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J13" s="1">
+      <c r="M13" s="1">
+        <v>18189</v>
+      </c>
+      <c r="N13" s="1">
+        <v>577</v>
+      </c>
+      <c r="O13" s="1">
+        <v>43</v>
+      </c>
+      <c r="P13" s="1">
+        <v>13990</v>
+      </c>
+      <c r="Q13" s="1">
+        <v>4</v>
+      </c>
+      <c r="R13" s="1">
+        <v>15</v>
+      </c>
+      <c r="S13" s="1">
+        <v>16</v>
+      </c>
+      <c r="T13" s="1">
         <v>2.84</v>
       </c>
     </row>
-    <row r="14" spans="2:10" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:20" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B14" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C14" s="1">
-        <v>3027</v>
+        <v>3163</v>
       </c>
       <c r="D14" s="1">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="E14" s="1">
         <v>15</v>
       </c>
       <c r="F14" s="1">
-        <v>555</v>
+        <v>560</v>
       </c>
       <c r="G14" s="1">
         <v>2</v>
@@ -926,47 +1219,101 @@
         <v>1</v>
       </c>
       <c r="J14" s="1">
+        <v>0.71</v>
+      </c>
+      <c r="L14" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M14" s="1">
+        <v>3027</v>
+      </c>
+      <c r="N14" s="1">
+        <v>70</v>
+      </c>
+      <c r="O14" s="1">
+        <v>15</v>
+      </c>
+      <c r="P14" s="1">
+        <v>555</v>
+      </c>
+      <c r="Q14" s="1">
+        <v>2</v>
+      </c>
+      <c r="R14" s="1">
+        <v>6</v>
+      </c>
+      <c r="S14" s="1">
+        <v>1</v>
+      </c>
+      <c r="T14" s="1">
         <v>1.27</v>
       </c>
     </row>
-    <row r="15" spans="2:10" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:20" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B15" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C15" s="1">
-        <v>10172</v>
+        <v>12621</v>
       </c>
       <c r="D15" s="1">
-        <v>327</v>
+        <v>434</v>
       </c>
       <c r="E15" s="1">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="F15" s="1">
-        <v>3113</v>
+        <v>5343</v>
       </c>
       <c r="G15" s="1">
         <v>4</v>
       </c>
       <c r="H15" s="1">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I15" s="1">
         <v>5</v>
       </c>
       <c r="J15" s="1">
+        <v>1.31</v>
+      </c>
+      <c r="L15" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="M15" s="1">
+        <v>10172</v>
+      </c>
+      <c r="N15" s="1">
+        <v>327</v>
+      </c>
+      <c r="O15" s="1">
+        <v>23</v>
+      </c>
+      <c r="P15" s="1">
+        <v>3113</v>
+      </c>
+      <c r="Q15" s="1">
+        <v>4</v>
+      </c>
+      <c r="R15" s="1">
+        <v>17</v>
+      </c>
+      <c r="S15" s="1">
+        <v>5</v>
+      </c>
+      <c r="T15" s="1">
         <v>1.61</v>
       </c>
     </row>
-    <row r="16" spans="2:10" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:20" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B16" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C16" s="1">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="D16" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E16" s="1">
         <v>22</v>
@@ -986,13 +1333,40 @@
       <c r="J16" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="2:10" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="L16" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M16" s="1">
+        <v>52</v>
+      </c>
+      <c r="N16" s="1">
+        <v>1</v>
+      </c>
+      <c r="O16" s="1">
+        <v>22</v>
+      </c>
+      <c r="P16" s="1">
+        <v>15</v>
+      </c>
+      <c r="Q16" s="1">
+        <v>0</v>
+      </c>
+      <c r="R16" s="1">
+        <v>0</v>
+      </c>
+      <c r="S16" s="1">
+        <v>0</v>
+      </c>
+      <c r="T16" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="2:20" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B17" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C17" s="1">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D17" s="1">
         <v>3</v>
@@ -1015,13 +1389,40 @@
       <c r="J17" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="2:10" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="L17" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M17" s="1">
+        <v>103</v>
+      </c>
+      <c r="N17" s="1">
+        <v>3</v>
+      </c>
+      <c r="O17" s="1">
+        <v>13</v>
+      </c>
+      <c r="P17" s="1">
+        <v>16</v>
+      </c>
+      <c r="Q17" s="1">
+        <v>0</v>
+      </c>
+      <c r="R17" s="1">
+        <v>0</v>
+      </c>
+      <c r="S17" s="1">
+        <v>0</v>
+      </c>
+      <c r="T17" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="2:20" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B18" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C18" s="5">
-        <v>787</v>
+        <v>792</v>
       </c>
       <c r="D18" s="5">
         <v>24</v>
@@ -1030,40 +1431,67 @@
         <v>38</v>
       </c>
       <c r="F18" s="5">
-        <v>480</v>
+        <v>477</v>
       </c>
       <c r="G18" s="5">
         <v>2</v>
       </c>
       <c r="H18" s="5">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I18" s="5">
         <v>1</v>
       </c>
-      <c r="J18" s="7">
+      <c r="J18" s="13">
+        <v>4.95</v>
+      </c>
+      <c r="L18" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="M18" s="5">
+        <v>787</v>
+      </c>
+      <c r="N18" s="5">
+        <v>24</v>
+      </c>
+      <c r="O18" s="5">
+        <v>38</v>
+      </c>
+      <c r="P18" s="5">
+        <v>480</v>
+      </c>
+      <c r="Q18" s="5">
+        <v>2</v>
+      </c>
+      <c r="R18" s="5">
+        <v>9</v>
+      </c>
+      <c r="S18" s="5">
+        <v>1</v>
+      </c>
+      <c r="T18" s="7">
         <v>5.13</v>
       </c>
     </row>
-    <row r="19" spans="2:10" ht="28" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="2:20" ht="28" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B19" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C19" s="8">
         <f>SUM(C6:C18)</f>
-        <v>50544</v>
+        <v>54050</v>
       </c>
       <c r="D19" s="8">
         <f>SUM(D6:D18)</f>
-        <v>1582</v>
+        <v>1712</v>
       </c>
       <c r="E19" s="9">
         <f>AVERAGE(E6:E18)</f>
-        <v>37.846153846153847</v>
+        <v>38.384615384615387</v>
       </c>
       <c r="F19" s="8">
         <f>SUM(F6:F18)</f>
-        <v>32264</v>
+        <v>34721</v>
       </c>
       <c r="G19" s="10">
         <f>AVERAGE(G6:G18)</f>
@@ -1071,14 +1499,49 @@
       </c>
       <c r="H19" s="10">
         <f>AVERAGE(H6:H18)</f>
-        <v>7.3076923076923075</v>
+        <v>7.0769230769230766</v>
       </c>
       <c r="I19" s="8">
         <f>SUM(I6:I18)</f>
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J19" s="10">
         <f>AVERAGE(J6:J18)</f>
+        <v>2.4730769230769232</v>
+      </c>
+      <c r="L19" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="M19" s="8">
+        <f>SUM(M6:M18)</f>
+        <v>50544</v>
+      </c>
+      <c r="N19" s="8">
+        <f>SUM(N6:N18)</f>
+        <v>1582</v>
+      </c>
+      <c r="O19" s="9">
+        <f>AVERAGE(O6:O18)</f>
+        <v>37.846153846153847</v>
+      </c>
+      <c r="P19" s="8">
+        <f>SUM(P6:P18)</f>
+        <v>32264</v>
+      </c>
+      <c r="Q19" s="10">
+        <f>AVERAGE(Q6:Q18)</f>
+        <v>1.8461538461538463</v>
+      </c>
+      <c r="R19" s="10">
+        <f>AVERAGE(R6:R18)</f>
+        <v>7.3076923076923075</v>
+      </c>
+      <c r="S19" s="8">
+        <f>SUM(S6:S18)</f>
+        <v>49</v>
+      </c>
+      <c r="T19" s="10">
+        <f>AVERAGE(T6:T18)</f>
         <v>2.5807692307692305</v>
       </c>
     </row>

</xml_diff>